<commit_message>
saving for now some errors running julia file
</commit_message>
<xml_diff>
--- a/Yarrowia-pretest-2-julia-io/Yarrowia_gp_pretest_2.xlsx
+++ b/Yarrowia-pretest-2-julia-io/Yarrowia_gp_pretest_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqkmuroi\gitcode\Yarrowia_media_optimizer\Yarrowia-pretest-2-julia-io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A26AF33-56EE-41C5-A7FE-DC29C97EF959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F18ABD-6602-48D0-B7E0-1534E2343B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16305" yWindow="-10815" windowWidth="16410" windowHeight="14145" xr2:uid="{8C085B71-5B87-4656-9DBC-023EADC8F59E}"/>
+    <workbookView xWindow="-16320" yWindow="-10935" windowWidth="16440" windowHeight="28320" xr2:uid="{8C085B71-5B87-4656-9DBC-023EADC8F59E}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="465">
   <si>
     <t>Compound</t>
   </si>
@@ -1394,6 +1394,45 @@
   </si>
   <si>
     <t>YAR_PT_2_80</t>
+  </si>
+  <si>
+    <t>ShorthandName</t>
+  </si>
+  <si>
+    <t>KI/Cu</t>
+  </si>
+  <si>
+    <t>Fe/Na/Co</t>
+  </si>
+  <si>
+    <t>Mg/Mn</t>
+  </si>
+  <si>
+    <t>V-mix</t>
+  </si>
+  <si>
+    <t>V-mix2</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Zn</t>
+  </si>
+  <si>
+    <t>Bor</t>
+  </si>
+  <si>
+    <t>Ino</t>
+  </si>
+  <si>
+    <t>Paba</t>
+  </si>
+  <si>
+    <t>Glu/NH</t>
+  </si>
+  <si>
+    <t>Buffer</t>
   </si>
 </sst>
 </file>
@@ -1772,10 +1811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F1F3C4-BFFD-495A-BC70-F91BDD9D00A4}">
-  <dimension ref="A1:CD13"/>
+  <dimension ref="A1:CE13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1786,2744 +1825,2777 @@
     <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>372</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>373</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>374</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>375</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>376</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>377</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>378</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>379</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>380</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>381</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>382</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>383</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>384</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>385</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>386</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>387</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>388</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>389</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>390</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>391</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>392</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>393</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>394</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>395</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>396</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>397</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>398</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>399</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>400</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>401</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>402</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>403</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>404</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>405</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>406</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>407</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>408</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>409</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>410</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>411</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>412</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>413</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>414</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>415</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>416</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>417</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>418</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>419</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>420</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>421</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>422</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>423</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>424</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>425</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>426</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>427</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>428</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>429</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>430</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>431</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>432</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>433</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>434</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>435</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>436</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>437</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>438</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>439</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>440</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>441</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>442</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>443</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>444</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>445</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>446</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>447</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>448</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>449</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>450</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>453</v>
+      </c>
+      <c r="C2">
         <v>4875</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1E-4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1.4377100698418499E-4</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1.21286053770802E-4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>2.1582783118811899E-4</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>1.32061625531728E-4</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>1.2025593573123601E-4</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>1.5754107097609599E-4</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>1.89620548277669E-4</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>1.8681397325402501E-4</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AL2">
+      <c r="AM2">
         <v>1.95739170100362E-4</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <v>2.0133078240223599E-4</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AT2">
+      <c r="AU2">
         <v>1.28041263121011E-4</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <v>1.1589249764825E-4</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BA2">
+      <c r="BB2">
         <v>1.48731509921433E-4</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BD2">
+      <c r="BE2">
         <v>1.04172753596445E-4</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BF2">
+      <c r="BG2">
         <v>1.7367947784236801E-4</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BH2" s="1" t="s">
+      <c r="BI2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BI2">
+      <c r="BJ2">
         <v>2.0990603713545901E-4</v>
       </c>
-      <c r="BJ2">
+      <c r="BK2">
         <v>1.38330735823006E-4</v>
       </c>
-      <c r="BK2" s="1" t="s">
+      <c r="BL2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BL2" s="1" t="s">
+      <c r="BM2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BM2">
+      <c r="BN2">
         <v>1.07709950449867E-4</v>
       </c>
-      <c r="BN2">
+      <c r="BO2">
         <v>1.54261496789898E-4</v>
       </c>
-      <c r="BO2">
+      <c r="BP2">
         <v>1.3325010475246201E-4</v>
       </c>
-      <c r="BP2">
+      <c r="BQ2">
         <v>1.0239200598008101E-4</v>
       </c>
-      <c r="BQ2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BR2">
+      <c r="BS2">
         <v>1.70881803798861E-4</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BT2" s="1" t="s">
+      <c r="BU2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BU2" s="1" t="s">
+      <c r="BV2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BV2" s="1" t="s">
+      <c r="BW2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BW2">
+      <c r="BX2">
         <v>1.7778171347712499E-4</v>
       </c>
-      <c r="BX2" s="1" t="s">
+      <c r="BY2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BY2" s="1" t="s">
+      <c r="BZ2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BZ2" s="1" t="s">
+      <c r="CA2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="CA2" s="1" t="s">
+      <c r="CB2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="CB2">
+      <c r="CC2">
         <v>1.6523103266447399E-4</v>
       </c>
-      <c r="CC2">
+      <c r="CD2">
         <v>1.10250780005699E-4</v>
       </c>
-      <c r="CD2" s="1" t="s">
+      <c r="CE2" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C3">
         <v>62662</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>4.26129104919827E-3</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>7.1319967093156598E-3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>4.4972605349513101E-3</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3.02924174482229E-3</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>3.0873002651620701E-3</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>3.16767495902213E-3</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>4.7311784187442597E-3</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>5.1448209799007799E-3</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>9.5075215891857103E-3</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>2.7494483124272601E-3</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>3.7095592840199199E-3</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>2.8856142107027802E-3</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>8.1247536659246992E-3</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>9.7671026239529099E-3</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>5.5358112723047602E-3</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>3.9325441455569403E-3</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>2.9635484347516E-3</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>5.2766775852221004E-3</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>3.49590633798613E-3</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>7.5138589430793204E-3</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>3.4040057324816902E-3</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>7.3588847877898503E-3</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>3.60257137884149E-3</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>5.4205955565538103E-3</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>6.7128804601871298E-3</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>4.6259112189056904E-3</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>5.8002557341701498E-3</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>8.7075612737008198E-3</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>4.9814243403326301E-3</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>6.8142760258439504E-3</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>3.5842002017583302E-3</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>9.1359224949175092E-3</v>
       </c>
-      <c r="AO3">
+      <c r="AP3">
         <v>6.4452487262220996E-3</v>
       </c>
-      <c r="AP3" s="1" t="s">
+      <c r="AQ3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>5.6507594978384501E-3</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>3.9665983451292698E-3</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>6.2204245531359099E-3</v>
       </c>
-      <c r="AT3">
+      <c r="AU3">
         <v>7.8622725078474603E-3</v>
       </c>
-      <c r="AU3" s="1" t="s">
+      <c r="AV3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <v>3.2944526058676601E-3</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>9.0146796292027501E-3</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <v>4.80997903950509E-3</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <v>3.8600043737436001E-3</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>8.0078637002881405E-3</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>4.0767930807689597E-3</v>
       </c>
-      <c r="BB3">
+      <c r="BC3">
         <v>3.3815490738517699E-3</v>
       </c>
-      <c r="BC3" s="1" t="s">
+      <c r="BD3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BD3">
+      <c r="BE3">
         <v>4.8644016009424E-3</v>
       </c>
-      <c r="BE3" s="1" t="s">
+      <c r="BF3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BF3">
+      <c r="BG3">
         <v>7.2374075124636197E-3</v>
       </c>
-      <c r="BG3">
+      <c r="BH3">
         <v>7.6290578768187303E-3</v>
       </c>
-      <c r="BH3">
+      <c r="BI3">
         <v>8.4214366829661203E-3</v>
       </c>
-      <c r="BI3" s="1" t="s">
+      <c r="BJ3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="BJ3">
+      <c r="BK3">
         <v>2.9324186172161302E-3</v>
       </c>
-      <c r="BK3">
+      <c r="BL3">
         <v>3.2428723089834599E-3</v>
       </c>
-      <c r="BL3">
+      <c r="BM3">
         <v>4.34109508601582E-3</v>
       </c>
-      <c r="BM3" s="1" t="s">
+      <c r="BN3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="BN3">
+      <c r="BO3">
         <v>9.8958929134681604E-3</v>
       </c>
-      <c r="BO3">
+      <c r="BP3">
         <v>5.0758139830845497E-3</v>
       </c>
-      <c r="BP3">
+      <c r="BQ3">
         <v>2.8245490010071601E-3</v>
       </c>
-      <c r="BQ3">
+      <c r="BR3">
         <v>8.3393657370613508E-3</v>
       </c>
-      <c r="BR3">
+      <c r="BS3">
         <v>3.7454476345555499E-3</v>
       </c>
-      <c r="BS3">
+      <c r="BT3">
         <v>5.8874208511522997E-3</v>
       </c>
-      <c r="BT3">
+      <c r="BU3">
         <v>6.5142736860046603E-3</v>
       </c>
-      <c r="BU3">
+      <c r="BV3">
         <v>6.0444969841816796E-3</v>
       </c>
-      <c r="BV3">
+      <c r="BW3">
         <v>5.6978385753198996E-3</v>
       </c>
-      <c r="BW3">
+      <c r="BX3">
         <v>6.3203312221643097E-3</v>
       </c>
-      <c r="BX3">
+      <c r="BY3">
         <v>6.9572448005666204E-3</v>
       </c>
-      <c r="BY3">
+      <c r="BZ3">
         <v>4.4231290789417104E-3</v>
       </c>
-      <c r="BZ3" s="1" t="s">
+      <c r="CA3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CA3">
+      <c r="CB3">
         <v>1.18095856497472E-2</v>
       </c>
-      <c r="CB3">
+      <c r="CC3">
         <v>9.3998675676838003E-3</v>
       </c>
-      <c r="CC3">
+      <c r="CD3">
         <v>4.13742858256364E-3</v>
       </c>
-      <c r="CD3">
+      <c r="CE3">
         <v>8.7405973060128497E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>455</v>
+      </c>
+      <c r="C4">
         <v>24843</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.45856590985913698</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.68511158352306301</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>0.31821669641008798</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>0.70272079220019001</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AJ4" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>0.39961255163869303</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AL4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AM4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AN4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AN4" s="1" t="s">
+      <c r="AO4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AO4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="AP4" s="1" t="s">
+      <c r="AQ4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AQ4" s="1" t="s">
+      <c r="AR4" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="AR4" s="1" t="s">
+      <c r="AS4" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AT4" s="1" t="s">
+      <c r="AU4" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AU4" s="1" t="s">
+      <c r="AV4" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AV4" s="1" t="s">
+      <c r="AW4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="AW4" s="1" t="s">
+      <c r="AX4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AX4" s="1" t="s">
+      <c r="AY4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AY4" s="1" t="s">
+      <c r="AZ4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AZ4" s="1" t="s">
+      <c r="BA4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="BA4" s="1" t="s">
+      <c r="BB4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="BB4" s="1" t="s">
+      <c r="BC4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="BC4" s="1" t="s">
+      <c r="BD4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="BD4" s="1" t="s">
+      <c r="BE4" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="BE4" s="1" t="s">
+      <c r="BF4" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="BF4" s="1" t="s">
+      <c r="BG4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="BG4" s="1" t="s">
+      <c r="BH4" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="BH4" s="1" t="s">
+      <c r="BI4" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BI4" s="1" t="s">
+      <c r="BJ4" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="BJ4" s="1" t="s">
+      <c r="BK4" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="BK4" s="1" t="s">
+      <c r="BL4" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="BL4" s="1" t="s">
+      <c r="BM4" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="BM4" s="1" t="s">
+      <c r="BN4" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="BN4" s="1" t="s">
+      <c r="BO4" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="BO4" s="1" t="s">
+      <c r="BP4" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="BP4" s="1" t="s">
+      <c r="BQ4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="BQ4" s="1" t="s">
+      <c r="BR4" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="BR4" s="1" t="s">
+      <c r="BS4" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="BS4" s="1" t="s">
+      <c r="BT4" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="BT4" s="1" t="s">
+      <c r="BU4" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="BU4" s="1" t="s">
+      <c r="BV4" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="BW4" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="BW4" s="1" t="s">
+      <c r="BX4" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="BX4" s="1" t="s">
+      <c r="BY4" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="BY4" s="1" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="BZ4" s="1" t="s">
+      <c r="CA4" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="CA4" s="1" t="s">
+      <c r="CB4" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="CB4" s="1" t="s">
+      <c r="CC4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="CC4" s="1" t="s">
+      <c r="CD4" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="CD4" s="1" t="s">
+      <c r="CE4" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C5">
         <v>938</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>1E-3</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>8.4835705229621E-4</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1.4926213494729499E-3</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>6.2035680258293096E-4</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>8.9756648345426298E-4</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1.22356253404393E-3</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>8.7570212264641105E-4</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>7.3681981863004396E-4</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>1.64170710563849E-3</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>1.01831926603112E-3</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1.4482874937069899E-3</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>1.2946712756272301E-3</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>7.5657189395211301E-4</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>1.08672976006666E-3</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>8.63907167900704E-4</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>7.1458747667158299E-4</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>5.5504670514110296E-4</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>9.3240081348952596E-4</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>4.8070710779957897E-4</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>1.1969222419886999E-3</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>7.5139533302207603E-4</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>4.57002091021231E-4</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>1.35179704620799E-3</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>1.0071364777394E-3</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>6.8211115731597698E-4</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>9.5492968850678195E-4</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>1.57316208041761E-3</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>1.3996107438373E-3</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>4.6823616618375601E-4</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>1.4133223728875299E-3</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>1.49611035306463E-3</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>7.6726022146231504E-4</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>9.7455281439265201E-4</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>1.4290349180795499E-3</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>5.3275717841039401E-4</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>8.0861060948557895E-4</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>5.67340513911209E-4</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>8.0417809316415197E-4</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>6.6593745070943095E-4</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>1.25240482720525E-3</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>8.3705980703941698E-4</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>1.14939683538905E-3</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>1.5498819213863499E-3</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>5.1723793337902797E-4</v>
       </c>
-      <c r="AU5">
+      <c r="AV5">
         <v>6.3256319419140801E-4</v>
       </c>
-      <c r="AV5">
+      <c r="AW5">
         <v>6.8514073481184103E-4</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <v>5.9583535414655796E-4</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>1.32386233520085E-3</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>7.1809454743902604E-4</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <v>1.10430133593506E-3</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <v>1.12893095925171E-3</v>
       </c>
-      <c r="BB5">
+      <c r="BC5">
         <v>5.2371326464756296E-4</v>
       </c>
-      <c r="BC5">
+      <c r="BD5">
         <v>1.24691975244805E-3</v>
       </c>
-      <c r="BD5">
+      <c r="BE5">
         <v>6.5780169710913101E-4</v>
       </c>
-      <c r="BE5">
+      <c r="BF5">
         <v>1.1675972856465E-3</v>
       </c>
-      <c r="BF5">
+      <c r="BG5">
         <v>4.7059235603830998E-4</v>
       </c>
-      <c r="BG5">
+      <c r="BH5">
         <v>5.72414699789815E-4</v>
       </c>
-      <c r="BH5">
+      <c r="BI5">
         <v>5.3602452063946705E-4</v>
       </c>
-      <c r="BI5">
+      <c r="BJ5">
         <v>4.8624515654187501E-4</v>
       </c>
-      <c r="BJ5">
+      <c r="BK5">
         <v>1.1776014064049001E-3</v>
       </c>
-      <c r="BK5">
+      <c r="BL5">
         <v>5.0926447769209502E-4</v>
       </c>
-      <c r="BL5">
+      <c r="BM5">
         <v>1.36980673589989E-3</v>
       </c>
-      <c r="BM5">
+      <c r="BN5">
         <v>8.3071197666213803E-4</v>
       </c>
-      <c r="BN5">
+      <c r="BO5">
         <v>9.0404883909241996E-4</v>
       </c>
-      <c r="BO5">
+      <c r="BP5">
         <v>1.06644678771372E-3</v>
       </c>
-      <c r="BP5">
+      <c r="BQ5">
         <v>7.0021263918517405E-4</v>
       </c>
-      <c r="BQ5">
+      <c r="BR5">
         <v>1.54260497289927E-3</v>
       </c>
-      <c r="BR5">
+      <c r="BS5">
         <v>6.1338991700185498E-4</v>
       </c>
-      <c r="BS5">
+      <c r="BT5">
         <v>9.8714635174919807E-4</v>
       </c>
-      <c r="BT5">
+      <c r="BU5">
         <v>1.0281271970729101E-3</v>
       </c>
-      <c r="BU5">
+      <c r="BV5">
         <v>1.0561732954450899E-3</v>
       </c>
-      <c r="BV5">
+      <c r="BW5">
         <v>5.4874216578234397E-4</v>
       </c>
-      <c r="BW5">
+      <c r="BX5">
         <v>6.0028603865597003E-4</v>
       </c>
-      <c r="BX5">
+      <c r="BY5">
         <v>6.5085572915004101E-4</v>
       </c>
-      <c r="BY5">
+      <c r="BZ5">
         <v>1.2718023911976999E-3</v>
       </c>
-      <c r="BZ5">
+      <c r="CA5">
         <v>4.9330034641583895E-4</v>
       </c>
-      <c r="CA5">
+      <c r="CB5">
         <v>9.2321303156583804E-4</v>
       </c>
-      <c r="CB5">
+      <c r="CC5">
         <v>7.8374596676940398E-4</v>
       </c>
-      <c r="CC5">
+      <c r="CD5">
         <v>5.8085907261737205E-4</v>
       </c>
-      <c r="CD5">
+      <c r="CE5">
         <v>1.62088795684124E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>457</v>
+      </c>
+      <c r="C6">
         <v>171548</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="AA6" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AC6" s="1" t="s">
+      <c r="AD6" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AF6" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AG6" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AG6" s="1" t="s">
+      <c r="AH6" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AH6" s="1" t="s">
+      <c r="AI6" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AJ6" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AJ6" s="1" t="s">
+      <c r="AK6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AK6" s="1" t="s">
+      <c r="AL6" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="AL6" s="1" t="s">
+      <c r="AM6" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AM6" s="1" t="s">
+      <c r="AN6" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="AN6" s="1" t="s">
+      <c r="AO6" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AO6" s="1" t="s">
+      <c r="AP6" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AP6" s="1" t="s">
+      <c r="AQ6" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AQ6" s="1" t="s">
+      <c r="AR6" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="AR6" s="1" t="s">
+      <c r="AS6" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="AS6" s="1" t="s">
+      <c r="AT6" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="AT6" s="1" t="s">
+      <c r="AU6" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="AU6" s="1" t="s">
+      <c r="AV6" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="AV6" s="1" t="s">
+      <c r="AW6" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="AW6" s="1" t="s">
+      <c r="AX6" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="AX6" s="1" t="s">
+      <c r="AY6" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="AY6" s="1" t="s">
+      <c r="AZ6" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="AZ6" s="1" t="s">
+      <c r="BA6" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="BA6" s="1" t="s">
+      <c r="BB6" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="BB6" s="1" t="s">
+      <c r="BC6" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="BC6" s="1" t="s">
+      <c r="BD6" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="BD6" s="1" t="s">
+      <c r="BE6" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="BE6" s="1" t="s">
+      <c r="BF6" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="BF6" s="1" t="s">
+      <c r="BG6" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="BG6" s="1" t="s">
+      <c r="BH6" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="BH6" s="1" t="s">
+      <c r="BI6" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="BI6" s="1" t="s">
+      <c r="BJ6" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="BJ6" s="1" t="s">
+      <c r="BK6" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="BK6" s="1" t="s">
+      <c r="BL6" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="BL6" s="1" t="s">
+      <c r="BM6" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="BM6" s="1" t="s">
+      <c r="BN6" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="BN6" s="1" t="s">
+      <c r="BO6" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="BO6" s="1" t="s">
+      <c r="BP6" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="BP6" s="1" t="s">
+      <c r="BQ6" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="BQ6" s="1" t="s">
+      <c r="BR6" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="BR6" s="1" t="s">
+      <c r="BS6" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="BS6" s="1" t="s">
+      <c r="BT6" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="BT6" s="1" t="s">
+      <c r="BU6" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="BU6" s="1" t="s">
+      <c r="BV6" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="BV6" s="1" t="s">
+      <c r="BW6" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="BW6" s="1" t="s">
+      <c r="BX6" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="BX6" s="1" t="s">
+      <c r="BY6" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="BY6" s="1" t="s">
+      <c r="BZ6" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="BZ6" s="1" t="s">
+      <c r="CA6" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="CA6" s="1" t="s">
+      <c r="CB6" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="CB6" s="1" t="s">
+      <c r="CC6" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="CC6" s="1" t="s">
+      <c r="CD6" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="CD6" s="1" t="s">
+      <c r="CE6" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>458</v>
+      </c>
+      <c r="C7">
         <v>6093260</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>8.1250000000000003E-3</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>7.9788301041464102E-2</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>9.5295019521687604E-2</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>3.6391425699764397E-2</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>7.5169064456223596E-3</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>6.1475584697314898E-3</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>4.3102468923474899E-2</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>8.64012965049131E-2</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>7.3689294145267106E-2</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>6.3861665108850399E-2</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>6.8639278414724496E-3</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>3.9037120086646102E-2</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>6.6237222992235698E-3</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>1.8609115567205299E-2</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>2.0594463521018101E-2</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AE7" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AF7" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="AF7">
+      <c r="AG7">
         <v>9.7976558986685905E-2</v>
       </c>
-      <c r="AG7" s="1" t="s">
+      <c r="AH7" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AI7" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="AI7">
+      <c r="AJ7">
         <v>2.0252419985896001E-2</v>
       </c>
-      <c r="AJ7" s="1" t="s">
+      <c r="AK7" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="AK7" s="1" t="s">
+      <c r="AL7" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AM7" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="AM7">
+      <c r="AN7">
         <v>9.0780033059965695E-3</v>
       </c>
-      <c r="AN7">
+      <c r="AO7">
         <v>8.4073727868702493E-3</v>
       </c>
-      <c r="AO7">
+      <c r="AP7">
         <v>8.01807575350914E-3</v>
       </c>
-      <c r="AP7">
+      <c r="AQ7">
         <v>6.9799913241046493E-2</v>
       </c>
-      <c r="AQ7" s="1" t="s">
+      <c r="AR7" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="AR7" s="1" t="s">
+      <c r="AS7" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="AS7" s="1" t="s">
+      <c r="AT7" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="AT7" s="1" t="s">
+      <c r="AU7" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="AU7">
+      <c r="AV7">
         <v>3.4428114992151801E-2</v>
       </c>
-      <c r="AV7" s="1" t="s">
+      <c r="AW7" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="AW7" s="1" t="s">
+      <c r="AX7" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="AX7" s="1" t="s">
+      <c r="AY7" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="AY7" s="1" t="s">
+      <c r="AZ7" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="AZ7" s="1" t="s">
+      <c r="BA7" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="BA7">
+      <c r="BB7">
         <v>5.96251827614473E-2</v>
       </c>
-      <c r="BB7" s="1" t="s">
+      <c r="BC7" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="BC7">
+      <c r="BD7">
         <v>6.7929543128140799E-2</v>
       </c>
-      <c r="BD7" s="1" t="s">
+      <c r="BE7" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="BE7">
+      <c r="BF7">
         <v>5.6992683985475003E-2</v>
       </c>
-      <c r="BF7">
+      <c r="BG7">
         <v>7.2152856919302502E-3</v>
       </c>
-      <c r="BG7">
+      <c r="BH7">
         <v>8.3102169261051601E-2</v>
       </c>
-      <c r="BH7">
+      <c r="BI7">
         <v>8.5083008267339503E-3</v>
       </c>
-      <c r="BI7">
+      <c r="BJ7">
         <v>1.9186096619741601E-2</v>
       </c>
-      <c r="BJ7" s="1" t="s">
+      <c r="BK7" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="BK7">
+      <c r="BL7">
         <v>4.3248350255185503E-2</v>
       </c>
-      <c r="BL7" s="1" t="s">
+      <c r="BM7" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="BM7" s="1" t="s">
+      <c r="BN7" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="BN7">
+      <c r="BO7">
         <v>9.8706995104233305E-3</v>
       </c>
-      <c r="BO7" s="1" t="s">
+      <c r="BP7" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="BP7" s="1" t="s">
+      <c r="BQ7" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="BQ7">
+      <c r="BR7">
         <v>5.5155253217742499E-2</v>
       </c>
-      <c r="BR7">
+      <c r="BS7">
         <v>2.1845319673025599E-2</v>
       </c>
-      <c r="BS7" s="1" t="s">
+      <c r="BT7" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="BT7" s="1" t="s">
+      <c r="BU7" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="BU7" s="1" t="s">
+      <c r="BV7" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="BV7">
+      <c r="BW7">
         <v>3.1271555728493799E-2</v>
       </c>
-      <c r="BW7" s="1" t="s">
+      <c r="BX7" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="BX7" s="1" t="s">
+      <c r="BY7" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="BY7">
+      <c r="BZ7">
         <v>7.4793357615486694E-2</v>
       </c>
-      <c r="BZ7">
+      <c r="CA7">
         <v>1.7710534045224099E-2</v>
       </c>
-      <c r="CA7">
+      <c r="CB7">
         <v>9.5526960573234093E-3</v>
       </c>
-      <c r="CB7">
+      <c r="CC7">
         <v>6.9732945571310502E-3</v>
       </c>
-      <c r="CC7">
+      <c r="CD7">
         <v>9.1379417204485003E-2</v>
       </c>
-      <c r="CD7" s="1" t="s">
+      <c r="CE7" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>459</v>
+      </c>
+      <c r="C8">
         <v>62640</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>6.7499999999999999E-3</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>9.3165989245489801E-4</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>4.6743589304717401E-4</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>2.25132999813991E-3</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>6.8714228996757996E-4</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>6.6539041553100803E-3</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>2.1624347059014102E-3</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>2.8272636640837802E-3</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>3.46292205437841E-3</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>7.8390927078204604E-4</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>9.7175704820062997E-4</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>7.9288761131147394E-3</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>6.3070210242727603E-3</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>1.3139757984794999E-2</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>2.4953630537360898E-3</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>1.642146077681E-3</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>1.3093342147184001E-3</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>7.3347497880879597E-4</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>5.4039259098455198E-4</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>7.6080078988553998E-3</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <v>6.7551195499100901E-3</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <v>9.9859606995183099E-3</v>
       </c>
-      <c r="AC8">
+      <c r="AD8">
         <v>5.0531573311645599E-4</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>1.58470226004155E-3</v>
       </c>
-      <c r="AE8">
+      <c r="AF8">
         <v>9.1026204746231E-3</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>5.1248935354143302E-3</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <v>1.0081615024386799E-3</v>
       </c>
-      <c r="AH8">
+      <c r="AI8">
         <v>3.0855817683111998E-3</v>
       </c>
-      <c r="AI8">
+      <c r="AJ8">
         <v>5.9825389867149796E-3</v>
       </c>
-      <c r="AJ8">
+      <c r="AK8">
         <v>3.1572918183378801E-3</v>
       </c>
-      <c r="AK8">
+      <c r="AL8">
         <v>1.3458969202344601E-3</v>
       </c>
-      <c r="AL8">
+      <c r="AM8">
         <v>9.6888479282453803E-3</v>
       </c>
-      <c r="AM8">
+      <c r="AN8">
         <v>3.9797984353390502E-4</v>
       </c>
-      <c r="AN8">
+      <c r="AO8">
         <v>3.7891379011469402E-3</v>
       </c>
-      <c r="AO8">
+      <c r="AP8">
         <v>1.20107892336555E-2</v>
       </c>
-      <c r="AP8">
+      <c r="AQ8">
         <v>4.13160157523987E-4</v>
       </c>
-      <c r="AQ8">
+      <c r="AR8">
         <v>1.3903643327412101E-3</v>
       </c>
-      <c r="AR8">
+      <c r="AS8">
         <v>4.7869023486807102E-3</v>
       </c>
-      <c r="AS8">
+      <c r="AT8">
         <v>7.2504264297406197E-3</v>
       </c>
-      <c r="AT8">
+      <c r="AU8">
         <v>4.9484685989364102E-3</v>
       </c>
-      <c r="AU8">
+      <c r="AV8">
         <v>1.2249043472001399E-3</v>
       </c>
-      <c r="AV8">
+      <c r="AW8">
         <v>4.58392014111234E-4</v>
       </c>
-      <c r="AW8">
+      <c r="AX8">
         <v>5.5188603487962302E-3</v>
       </c>
-      <c r="AX8">
+      <c r="AY8">
         <v>5.1145508536663701E-4</v>
       </c>
-      <c r="AY8">
+      <c r="AZ8">
         <v>1.7703054036602201E-3</v>
       </c>
-      <c r="AZ8">
+      <c r="BA8">
         <v>1.0971866781881901E-3</v>
       </c>
-      <c r="BA8">
+      <c r="BB8">
         <v>6.4364944432607402E-4</v>
       </c>
-      <c r="BB8">
+      <c r="BC8">
         <v>3.7871007324797099E-4</v>
       </c>
-      <c r="BC8">
+      <c r="BD8">
         <v>7.6020556505867196E-4</v>
       </c>
-      <c r="BD8">
+      <c r="BE8">
         <v>1.0809044882990101E-3</v>
       </c>
-      <c r="BE8">
+      <c r="BF8">
         <v>8.8391832304590603E-3</v>
       </c>
-      <c r="BF8">
+      <c r="BG8">
         <v>1.2750631610632701E-2</v>
       </c>
-      <c r="BG8">
+      <c r="BH8">
         <v>2.0662101857192501E-3</v>
       </c>
-      <c r="BH8" s="1" t="s">
+      <c r="BI8" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="BI8">
+      <c r="BJ8">
         <v>8.7826642498666397E-4</v>
       </c>
-      <c r="BJ8">
+      <c r="BK8">
         <v>2.6276343175169899E-3</v>
       </c>
-      <c r="BK8">
+      <c r="BL8">
         <v>4.3533304613321898E-4</v>
       </c>
-      <c r="BL8">
+      <c r="BM8">
         <v>1.1629298363592399E-3</v>
       </c>
-      <c r="BM8">
+      <c r="BN8">
         <v>2.45497958648371E-3</v>
       </c>
-      <c r="BN8">
+      <c r="BO8">
         <v>6.5472504402625605E-4</v>
       </c>
-      <c r="BO8">
+      <c r="BP8">
         <v>3.3632711539535302E-3</v>
       </c>
-      <c r="BP8">
+      <c r="BQ8">
         <v>1.68921108097715E-3</v>
       </c>
-      <c r="BQ8">
+      <c r="BR8">
         <v>1.94999873027521E-3</v>
       </c>
-      <c r="BR8">
+      <c r="BS8">
         <v>5.6108480428048004E-3</v>
       </c>
-      <c r="BS8">
+      <c r="BT8">
         <v>8.1570403104635099E-3</v>
       </c>
-      <c r="BT8">
+      <c r="BU8">
         <v>6.0697148524436497E-4</v>
       </c>
-      <c r="BU8">
+      <c r="BV8">
         <v>3.69807057412982E-3</v>
       </c>
-      <c r="BV8">
+      <c r="BW8">
         <v>4.3415846157801004E-3</v>
       </c>
-      <c r="BW8">
+      <c r="BX8">
         <v>5.7690600336745505E-4</v>
       </c>
-      <c r="BX8">
+      <c r="BY8">
         <v>4.3845836606622004E-3</v>
       </c>
-      <c r="BY8">
+      <c r="BZ8">
         <v>2.9156296868422002E-3</v>
       </c>
-      <c r="BZ8">
+      <c r="CA8">
         <v>1.47920389924463E-3</v>
       </c>
-      <c r="CA8" s="1" t="s">
+      <c r="CB8" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="CB8">
+      <c r="CC8">
         <v>8.4628222439220497E-4</v>
       </c>
-      <c r="CC8">
+      <c r="CD8">
         <v>4.0875069059275303E-3</v>
       </c>
-      <c r="CD8">
+      <c r="CE8">
         <v>1.8527007189945101E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>460</v>
+      </c>
+      <c r="C9">
         <v>7628</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1E-3</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>5.4773284806217105E-4</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>5.0862219755464996E-4</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1.0758232274557999E-3</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>5.9396985065122705E-4</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>5.5627742322990098E-4</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1.3995169910358E-3</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>5.2577856825101901E-4</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>1.50398236837032E-3</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>1.3339269001626001E-3</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>1.01853395036573E-3</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>2.1910790106941698E-3</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>2.0791187587277998E-3</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>1.35109107201103E-3</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>1.9543404187462301E-3</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>6.6023927240447904E-4</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>1.8279483091675501E-3</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>4.9959414332779496E-4</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>9.3395114733991005E-4</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>1.1816440598423101E-3</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>6.7320020041234101E-4</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>7.99351000238204E-4</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>1.6428154051880001E-3</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>6.8270227947915497E-4</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>1.7433575369377599E-3</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>5.7199912260176295E-4</v>
       </c>
-      <c r="AC9">
+      <c r="AD9">
         <v>8.4494932422936797E-4</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>1.36801329166278E-3</v>
       </c>
-      <c r="AE9">
+      <c r="AF9">
         <v>1.8508045007857E-3</v>
       </c>
-      <c r="AF9">
+      <c r="AG9">
         <v>7.4184853849040995E-4</v>
       </c>
-      <c r="AG9">
+      <c r="AH9">
         <v>6.4212140882566305E-4</v>
       </c>
-      <c r="AH9">
+      <c r="AI9">
         <v>8.6444368716305205E-4</v>
       </c>
-      <c r="AI9">
+      <c r="AJ9">
         <v>1.89347840407274E-3</v>
       </c>
-      <c r="AJ9">
+      <c r="AK9">
         <v>1.5783291098223099E-3</v>
       </c>
-      <c r="AK9">
+      <c r="AL9">
         <v>4.7613133565476898E-4</v>
       </c>
-      <c r="AL9">
+      <c r="AM9">
         <v>9.1634403990924901E-4</v>
       </c>
-      <c r="AM9">
+      <c r="AN9">
         <v>8.1811229748942303E-4</v>
       </c>
-      <c r="AN9">
+      <c r="AO9">
         <v>1.9952801654104899E-3</v>
       </c>
-      <c r="AO9">
+      <c r="AP9">
         <v>1.44257208780518E-3</v>
       </c>
-      <c r="AP9">
+      <c r="AQ9">
         <v>7.6801792639490097E-4</v>
       </c>
-      <c r="AQ9">
+      <c r="AR9">
         <v>6.1020268730853095E-4</v>
       </c>
-      <c r="AR9">
+      <c r="AS9">
         <v>5.7961280269897897E-4</v>
       </c>
-      <c r="AS9">
+      <c r="AT9">
         <v>6.2370537302492801E-4</v>
       </c>
-      <c r="AT9">
+      <c r="AU9">
         <v>7.4989314583022101E-4</v>
       </c>
-      <c r="AU9">
+      <c r="AV9">
         <v>1.2962733044033299E-3</v>
       </c>
-      <c r="AV9">
+      <c r="AW9">
         <v>8.7940675354584096E-4</v>
       </c>
-      <c r="AW9">
+      <c r="AX9">
         <v>1.0703736359738299E-3</v>
       </c>
-      <c r="AX9">
+      <c r="AY9">
         <v>1.2762497583286799E-3</v>
       </c>
-      <c r="AY9">
+      <c r="AZ9">
         <v>2.12592724126237E-3</v>
       </c>
-      <c r="AZ9">
+      <c r="BA9">
         <v>1.25634732458048E-3</v>
       </c>
-      <c r="BA9">
+      <c r="BB9">
         <v>1.1425099147211199E-3</v>
       </c>
-      <c r="BB9">
+      <c r="BC9">
         <v>8.4032083785393096E-4</v>
       </c>
-      <c r="BC9">
+      <c r="BD9">
         <v>1.00749950993452E-3</v>
       </c>
-      <c r="BD9">
+      <c r="BE9">
         <v>7.2172670079226201E-4</v>
       </c>
-      <c r="BE9">
+      <c r="BF9">
         <v>1.50722466686286E-3</v>
       </c>
-      <c r="BF9">
+      <c r="BG9">
         <v>4.6643968957551699E-4</v>
       </c>
-      <c r="BG9">
+      <c r="BH9">
         <v>1.60718282104711E-3</v>
       </c>
-      <c r="BH9">
+      <c r="BI9">
         <v>5.1817859536585405E-4</v>
       </c>
-      <c r="BI9">
+      <c r="BJ9">
         <v>1.67195535717234E-3</v>
       </c>
-      <c r="BJ9">
+      <c r="BK9">
         <v>5.3614999079788696E-4</v>
       </c>
-      <c r="BK9">
+      <c r="BL9">
         <v>1.4501570661724899E-3</v>
       </c>
-      <c r="BL9">
+      <c r="BM9">
         <v>1.7114279790619101E-3</v>
       </c>
-      <c r="BM9">
+      <c r="BN9">
         <v>4.8931223491378102E-4</v>
       </c>
-      <c r="BN9">
+      <c r="BO9">
         <v>6.9282414482737804E-4</v>
       </c>
-      <c r="BO9">
+      <c r="BP9">
         <v>7.1436118633829901E-4</v>
       </c>
-      <c r="BP9">
+      <c r="BQ9">
         <v>9.5319314564422299E-4</v>
       </c>
-      <c r="BQ9">
+      <c r="BR9">
         <v>1.5517179112720901E-3</v>
       </c>
-      <c r="BR9">
+      <c r="BS9">
         <v>1.19128611712609E-3</v>
       </c>
-      <c r="BS9">
+      <c r="BT9">
         <v>1.9133777048668001E-3</v>
       </c>
-      <c r="BT9">
+      <c r="BU9">
         <v>2.03620068248521E-3</v>
       </c>
-      <c r="BU9">
+      <c r="BV9">
         <v>1.12946919416061E-3</v>
       </c>
-      <c r="BV9">
+      <c r="BW9">
         <v>8.9934649065820502E-4</v>
       </c>
-      <c r="BW9">
+      <c r="BX9">
         <v>6.2689471063617503E-4</v>
       </c>
-      <c r="BX9">
+      <c r="BY9">
         <v>9.8371706029117597E-4</v>
       </c>
-      <c r="BY9">
+      <c r="BZ9">
         <v>4.6310327524064899E-4</v>
       </c>
-      <c r="BZ9">
+      <c r="CA9">
         <v>1.7705487504454101E-3</v>
       </c>
-      <c r="CA9">
+      <c r="CB9">
         <v>1.03871095682194E-3</v>
       </c>
-      <c r="CB9">
+      <c r="CC9">
         <v>7.8826449255001098E-4</v>
       </c>
-      <c r="CC9">
+      <c r="CD9">
         <v>1.21295419069816E-3</v>
       </c>
-      <c r="CD9">
+      <c r="CE9">
         <v>1.09969987911876E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C10">
         <v>892</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>3.3569148278046898E-2</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>1.4786802735814499E-4</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>6.09791191923836E-3</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>3.8624046469333702E-4</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>1.02559853727637E-4</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>1.2905775328963799E-4</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>1.9121333305896401E-4</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>1.0591156873657501E-3</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>9.2267059176381495E-3</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>5.7104600560821102E-4</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="Y10" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="Y10" s="1" t="s">
+      <c r="Z10" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="Z10" s="1" t="s">
+      <c r="AA10" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AB10" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="AB10" s="1" t="s">
+      <c r="AC10" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>9.3999747214704903E-4</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>1.3185826059300299E-3</v>
       </c>
-      <c r="AE10">
+      <c r="AF10">
         <v>1.06371878470037E-4</v>
       </c>
-      <c r="AF10" s="1" t="s">
+      <c r="AG10" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <v>3.63101658524806E-3</v>
       </c>
-      <c r="AH10">
+      <c r="AI10">
         <v>7.9462551403709704E-4</v>
       </c>
-      <c r="AI10" s="1" t="s">
+      <c r="AJ10" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="AJ10">
+      <c r="AK10">
         <v>3.94348273546564E-2</v>
       </c>
-      <c r="AK10">
+      <c r="AL10">
         <v>4.5816830193268698E-4</v>
       </c>
-      <c r="AL10" s="1" t="s">
+      <c r="AM10" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="AM10">
+      <c r="AN10">
         <v>8.31384765495518E-4</v>
       </c>
-      <c r="AN10">
+      <c r="AO10">
         <v>3.24344272864088E-4</v>
       </c>
-      <c r="AO10" s="1" t="s">
+      <c r="AP10" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="AP10" s="1" t="s">
+      <c r="AQ10" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="AQ10" s="1" t="s">
+      <c r="AR10" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="AR10">
+      <c r="AS10">
         <v>6.4172340233180497E-3</v>
       </c>
-      <c r="AS10" s="1" t="s">
+      <c r="AT10" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AT10" s="1" t="s">
+      <c r="AU10" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="AU10">
+      <c r="AV10">
         <v>2.5734061752918399E-3</v>
       </c>
-      <c r="AV10" s="1" t="s">
+      <c r="AW10" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="AW10">
+      <c r="AX10">
         <v>2.1514730164364499E-4</v>
       </c>
-      <c r="AX10" s="1" t="s">
+      <c r="AY10" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="AY10">
+      <c r="AZ10">
         <v>5.2110955217346696E-4</v>
       </c>
-      <c r="AZ10">
+      <c r="BA10">
         <v>2.6445342335880401E-4</v>
       </c>
-      <c r="BA10">
+      <c r="BB10">
         <v>3.9268632974513596E-3</v>
       </c>
-      <c r="BB10">
+      <c r="BC10">
         <v>2.3664071618592001E-3</v>
       </c>
-      <c r="BC10" s="1" t="s">
+      <c r="BD10" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="BD10" s="1" t="s">
+      <c r="BE10" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="BE10">
+      <c r="BF10">
         <v>1.67874479103846E-3</v>
       </c>
-      <c r="BF10">
+      <c r="BG10">
         <v>1.38012579196873E-3</v>
       </c>
-      <c r="BG10" s="1" t="s">
+      <c r="BH10" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="BH10">
+      <c r="BI10">
         <v>2.4044770360596201E-4</v>
       </c>
-      <c r="BI10" s="1" t="s">
+      <c r="BJ10" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="BJ10">
+      <c r="BK10">
         <v>8.1808715686353499E-3</v>
       </c>
-      <c r="BK10" s="1" t="s">
+      <c r="BL10" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="BL10">
+      <c r="BM10">
         <v>1.59577398225869E-4</v>
       </c>
-      <c r="BM10">
+      <c r="BN10">
         <v>4.45019023529746E-3</v>
       </c>
-      <c r="BN10">
+      <c r="BO10">
         <v>1.64412933522807E-2</v>
       </c>
-      <c r="BO10" s="1" t="s">
+      <c r="BP10" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="BP10">
+      <c r="BQ10">
         <v>6.3235190689085404E-4</v>
       </c>
-      <c r="BQ10" s="1" t="s">
+      <c r="BR10" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="BR10" s="1" t="s">
+      <c r="BS10" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="BS10" s="1" t="s">
+      <c r="BT10" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="BT10">
+      <c r="BU10">
         <v>3.17539647417401E-3</v>
       </c>
-      <c r="BU10" s="1" t="s">
+      <c r="BV10" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="BV10">
+      <c r="BW10">
         <v>3.7599360104489601E-4</v>
       </c>
-      <c r="BW10">
+      <c r="BX10">
         <v>5.2251318853705399E-3</v>
       </c>
-      <c r="BX10" s="1" t="s">
+      <c r="BY10" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="BY10" s="1" t="s">
+      <c r="BZ10" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="BZ10">
+      <c r="CA10">
         <v>7.58710309784445E-3</v>
       </c>
-      <c r="CA10" s="1" t="s">
+      <c r="CB10" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="CB10">
+      <c r="CC10">
         <v>1.1641819923232001E-2</v>
       </c>
-      <c r="CC10">
+      <c r="CD10">
         <v>1.8400279227504101E-3</v>
       </c>
-      <c r="CD10">
+      <c r="CE10">
         <v>2.19927757318388E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>462</v>
+      </c>
+      <c r="C11">
         <v>978</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>1E-4</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>1.1999550533896E-4</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>1.4509212747940199E-4</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>1.11557564045316E-4</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>2.0787012702442199E-4</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>1.5793439141766801E-4</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>2.1849048694049401E-4</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>1.09719981957648E-4</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>1.00937956853477E-4</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>1.75479492780763E-4</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="X11" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>1.8278152615737599E-4</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>1.05769200328783E-4</v>
       </c>
-      <c r="Z11" s="1" t="s">
+      <c r="AA11" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="AB11" s="1" t="s">
+      <c r="AC11" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="AC11" s="1" t="s">
+      <c r="AD11" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AE11" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="AE11" s="1" t="s">
+      <c r="AF11" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="AF11" s="1" t="s">
+      <c r="AG11" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="AG11" s="1" t="s">
+      <c r="AH11" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="AH11">
+      <c r="AI11">
         <v>1.8867201534783501E-4</v>
       </c>
-      <c r="AI11">
+      <c r="AJ11">
         <v>1.3892165043649399E-4</v>
       </c>
-      <c r="AJ11">
+      <c r="AK11">
         <v>1.1911387424841E-4</v>
       </c>
-      <c r="AK11" s="1" t="s">
+      <c r="AL11" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="AL11" s="1" t="s">
+      <c r="AM11" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="AM11">
+      <c r="AN11">
         <v>1.4368217876758099E-4</v>
       </c>
-      <c r="AN11" s="1" t="s">
+      <c r="AO11" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="AO11">
+      <c r="AP11">
         <v>1.98300434437249E-4</v>
       </c>
-      <c r="AP11">
+      <c r="AQ11">
         <v>2.1027368802272901E-4</v>
       </c>
-      <c r="AQ11" s="1" t="s">
+      <c r="AR11" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="AR11" s="1" t="s">
+      <c r="AS11" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="AS11" s="1" t="s">
+      <c r="AT11" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="AT11">
+      <c r="AU11">
         <v>1.2734571323083901E-4</v>
       </c>
-      <c r="AU11" s="1" t="s">
+      <c r="AV11" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="AV11" s="1" t="s">
+      <c r="AW11" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="AW11" s="1" t="s">
+      <c r="AX11" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="AX11" s="1" t="s">
+      <c r="AY11" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="AY11" s="1" t="s">
+      <c r="AZ11" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="AZ11" s="1" t="s">
+      <c r="BA11" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="BA11" s="1" t="s">
+      <c r="BB11" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="BB11" s="1" t="s">
+      <c r="BC11" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="BC11" s="1" t="s">
+      <c r="BD11" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="BD11" s="1" t="s">
+      <c r="BE11" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="BE11" s="1" t="s">
+      <c r="BF11" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="BF11">
+      <c r="BG11">
         <v>1.3570362691899199E-4</v>
       </c>
-      <c r="BG11">
+      <c r="BH11">
         <v>1.2551672326527501E-4</v>
       </c>
-      <c r="BH11" s="1" t="s">
+      <c r="BI11" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="BI11">
+      <c r="BJ11">
         <v>1.4940499514511899E-4</v>
       </c>
-      <c r="BJ11" s="1" t="s">
+      <c r="BK11" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="BK11" s="1" t="s">
+      <c r="BL11" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="BL11" s="1" t="s">
+      <c r="BM11" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="BM11" s="1" t="s">
+      <c r="BN11" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="BN11" s="1" t="s">
+      <c r="BO11" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="BO11" s="1" t="s">
+      <c r="BP11" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="BP11" s="1" t="s">
+      <c r="BQ11" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="BQ11">
+      <c r="BR11">
         <v>1.0228612518596101E-4</v>
       </c>
-      <c r="BR11">
+      <c r="BS11">
         <v>1.30758909350818E-4</v>
       </c>
-      <c r="BS11">
+      <c r="BT11">
         <v>1.6940284019125601E-4</v>
       </c>
-      <c r="BT11">
+      <c r="BU11">
         <v>1.8480490935966499E-4</v>
       </c>
-      <c r="BU11">
+      <c r="BV11">
         <v>1.9768754882382199E-4</v>
       </c>
-      <c r="BV11" s="1" t="s">
+      <c r="BW11" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="BW11" s="1" t="s">
+      <c r="BX11" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="BX11" s="1" t="s">
+      <c r="BY11" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="BY11">
+      <c r="BZ11">
         <v>1.14253060576877E-4</v>
       </c>
-      <c r="BZ11">
+      <c r="CA11">
         <v>1.64797281353946E-4</v>
       </c>
-      <c r="CA11">
+      <c r="CB11">
         <v>1.5225961294789599E-4</v>
       </c>
-      <c r="CB11" s="1" t="s">
+      <c r="CC11" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="CC11">
+      <c r="CD11">
         <v>1.6044462333218899E-4</v>
       </c>
-      <c r="CD11" s="1" t="s">
+      <c r="CE11" s="1" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>463</v>
+      </c>
+      <c r="C12">
         <v>5793</v>
       </c>
-      <c r="C12">
-        <v>20</v>
-      </c>
       <c r="D12">
         <v>20</v>
       </c>
@@ -4761,17 +4833,20 @@
       <c r="CD12">
         <v>20</v>
       </c>
+      <c r="CE12">
+        <v>20</v>
+      </c>
     </row>
-    <row r="13" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>464</v>
+      </c>
+      <c r="C13">
         <v>6096963</v>
       </c>
-      <c r="C13">
-        <v>9.5790000000000006</v>
-      </c>
       <c r="D13">
         <v>9.5790000000000006</v>
       </c>
@@ -5007,6 +5082,9 @@
         <v>9.5790000000000006</v>
       </c>
       <c r="CD13">
+        <v>9.5790000000000006</v>
+      </c>
+      <c r="CE13">
         <v>9.5790000000000006</v>
       </c>
     </row>

</xml_diff>